<commit_message>
Long press on the button implemented
With LEDs loading effect
</commit_message>
<xml_diff>
--- a/Datasheets/Parts.xlsx
+++ b/Datasheets/Parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolashippert/Documents/GitHub/ComplimentGenerator/Datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23D261F6-E8A6-774A-A538-E667CA9688B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5C2C62-1E3B-354F-8200-AB1BEE3F510F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{42112BD5-6223-2544-97F7-7501DEE01312}"/>
+    <workbookView xWindow="43220" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{42112BD5-6223-2544-97F7-7501DEE01312}"/>
   </bookViews>
   <sheets>
     <sheet name="Nomenclature" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Part</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Ultrasonic sensor</t>
+  </si>
+  <si>
+    <t>Schema reference</t>
   </si>
 </sst>
 </file>
@@ -430,109 +433,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827FF1F6-9EA8-E144-A881-2670B2D9E26E}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="F4">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>4</v>
       </c>
     </row>

</xml_diff>